<commit_message>
Update 'Casos de prueba.xlsx'
</commit_message>
<xml_diff>
--- a/project/Casos de prueba.xlsx
+++ b/project/Casos de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Desktop\Entrega Final\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAC1CFB-FC64-4C5A-891A-F2CAA0598999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C4DCBC-E2D2-44DA-B066-3C2DA372BCD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -170,6 +170,54 @@
   </si>
   <si>
     <t>Autenticacion de Usuarios (Log In)</t>
+  </si>
+  <si>
+    <t>Al registrar un usuario, este se guarda en la base de datos con todos los datos ingresados correspondientes. Se lo debe redirigir al inicio y autenticarlo</t>
+  </si>
+  <si>
+    <t>Se guarda el usuario correctamente en la base de datos. Redirige a inicio autenticandolo</t>
+  </si>
+  <si>
+    <t>Autentica el usuario si las credenciales ingresadas son validas y coinciden. Redirige a inicio</t>
+  </si>
+  <si>
+    <t>Atuentica el usuario correctamente si se cumplen las condiciones. Redirige a inicio</t>
+  </si>
+  <si>
+    <t>Modificacion de datos del usuario</t>
+  </si>
+  <si>
+    <t>Modifica los datos ingresados en el formulario cuando corresponda. Redirige a inicio, con el usuario autenticado</t>
+  </si>
+  <si>
+    <t>Modifica exitosamente los datos del usuario. Redirige a inicio y la autenticacion se mantiene</t>
+  </si>
+  <si>
+    <t>Modificacion de contraseña</t>
+  </si>
+  <si>
+    <t>Modifica la contraseña del usuario si los datos ingresados son validos y coinciden. Redirige a inicio y desautentica al usuario de su sesion</t>
+  </si>
+  <si>
+    <t>Modifica exitosamente la contraseña del usuario. Redirige a inicio y desautentica correctamente al usuario de su sesion.</t>
+  </si>
+  <si>
+    <t>Establecer avatar</t>
+  </si>
+  <si>
+    <t>Establece el avatar seleccionado por el usuario a la cuenta del mismo. De no poseer uno, se mostrara la imagen predeterminada como foto de perfil.</t>
+  </si>
+  <si>
+    <t>Establece correctamente la imagen seleccionada como el avatar del usuario.</t>
+  </si>
+  <si>
+    <t>Editar avatar</t>
+  </si>
+  <si>
+    <t>Edita el avatar seleccionado, reemplazando el anterior por el nuevo. La vista de editar muestra el avatar actual que posee el usuario</t>
+  </si>
+  <si>
+    <t>Edita exitosamente el avatar. Muestra correctamente la foto de perfil actual del usuario</t>
   </si>
 </sst>
 </file>
@@ -521,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -854,59 +902,121 @@
       <c r="A16" s="6">
         <v>10</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="11">
+        <v>45035</v>
+      </c>
       <c r="C16" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="6"/>
+      <c r="D16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>11</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="11">
+        <v>45035</v>
+      </c>
       <c r="C17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="6"/>
+      <c r="D17" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>12</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="6"/>
+      <c r="B18" s="11">
+        <v>45035</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="6"/>
+    <row r="19" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>13</v>
+      </c>
+      <c r="B19" s="11">
+        <v>45035</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="6"/>
+    <row r="20" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>14</v>
+      </c>
+      <c r="B20" s="11">
+        <v>45035</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="6"/>
+    <row r="21" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>15</v>
+      </c>
+      <c r="B21" s="11">
+        <v>45035</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>